<commit_message>
fixed linked to filter
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFull.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/UsersFull.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5574" uniqueCount="2493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5574" uniqueCount="2508">
   <si>
     <t>A</t>
   </si>
@@ -7512,6 +7512,51 @@
   </si>
   <si>
     <t>lhellens@med.cornell.edu</t>
+  </si>
+  <si>
+    <t>Weill Cornell Medical College;Weill Cornell Medical College</t>
+  </si>
+  <si>
+    <t>Pathology Informatics;Pathology Informatics</t>
+  </si>
+  <si>
+    <t>Billing and Compliance;Billing and Compliance</t>
+  </si>
+  <si>
+    <t>Anatomic Pathology;Anatomic Pathology</t>
+  </si>
+  <si>
+    <t>Genitourinary Pathology;Genitourinary Pathology</t>
+  </si>
+  <si>
+    <t>Research;Research</t>
+  </si>
+  <si>
+    <t>Renal Pathology;Renal Pathology</t>
+  </si>
+  <si>
+    <t>New York-Presbyterian Hospital;New York-Presbyterian Hospital;New York-Presbyterian Hospital</t>
+  </si>
+  <si>
+    <t>Pathology and Laboratory Medicine;Pathology and Laboratory Medicine;Pathology and Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>Hematopathology;Hematopathology;Hematopathology</t>
+  </si>
+  <si>
+    <t>New York-Presbyterian Hospital;New York-Presbyterian Hospital</t>
+  </si>
+  <si>
+    <t>Laboratory Medicine;Laboratory Medicine</t>
+  </si>
+  <si>
+    <t>Central Laboratory;Central Laboratory</t>
+  </si>
+  <si>
+    <t>NYP Lower Manhattan Hospital;NYP Lower Manhattan Hospital</t>
+  </si>
+  <si>
+    <t>NYP Lower Manhattan Hospital Laboratory;NYP Lower Manhattan Hospital Laboratory</t>
   </si>
 </sst>
 </file>
@@ -9877,10 +9922,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C152" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C182" workbookViewId="0">
       <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="C89" sqref="C89"/>
-      <selection pane="topRight" activeCell="AF159" sqref="AF159"/>
+      <selection pane="topRight" activeCell="K187" sqref="K187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -12308,7 +12353,7 @@
       <c r="BK23" s="62"/>
       <c r="BL23" s="42"/>
     </row>
-    <row r="24" spans="1:64" s="1" customFormat="1" ht="45">
+    <row r="24" spans="1:64" s="1" customFormat="1" ht="75">
       <c r="A24" s="7" t="b">
         <v>0</v>
       </c>
@@ -12329,13 +12374,13 @@
         <v>1271</v>
       </c>
       <c r="J24" s="42" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>1015</v>
+        <v>2494</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
@@ -15672,7 +15717,7 @@
       <c r="BK58" s="62"/>
       <c r="BL58" s="42"/>
     </row>
-    <row r="59" spans="1:64" s="1" customFormat="1" ht="45">
+    <row r="59" spans="1:64" s="1" customFormat="1" ht="75">
       <c r="A59" s="7" t="b">
         <v>1</v>
       </c>
@@ -15693,16 +15738,16 @@
         <v>1517</v>
       </c>
       <c r="J59" s="39" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>769</v>
+        <v>2496</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>177</v>
+        <v>2499</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="5"/>
@@ -18781,7 +18826,7 @@
       <c r="BK90" s="62"/>
       <c r="BL90" s="42"/>
     </row>
-    <row r="91" spans="1:64" s="1" customFormat="1" ht="60">
+    <row r="91" spans="1:64" s="1" customFormat="1" ht="75">
       <c r="A91" s="7" t="b">
         <v>0</v>
       </c>
@@ -18802,13 +18847,13 @@
         <v>1283</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="L91" s="5" t="s">
-        <v>285</v>
+        <v>2495</v>
       </c>
       <c r="M91" s="5"/>
       <c r="N91" s="5"/>
@@ -19004,13 +19049,13 @@
         <v>835</v>
       </c>
       <c r="AB93" s="42" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="AC93" s="42" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="AD93" s="42" t="s">
-        <v>533</v>
+        <v>2498</v>
       </c>
       <c r="AE93" s="42"/>
       <c r="AF93" s="5" t="s">
@@ -22711,13 +22756,13 @@
         <v>969</v>
       </c>
       <c r="AB131" s="42" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="AC131" s="42" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="AD131" s="42" t="s">
-        <v>533</v>
+        <v>2498</v>
       </c>
       <c r="AE131" s="42"/>
       <c r="AF131" s="5" t="s">
@@ -25565,16 +25610,16 @@
         <v>1854</v>
       </c>
       <c r="J159" s="39" t="s">
-        <v>1215</v>
+        <v>2500</v>
       </c>
       <c r="K159" s="5" t="s">
-        <v>776</v>
+        <v>2501</v>
       </c>
       <c r="L159" s="5" t="s">
-        <v>411</v>
+        <v>2502</v>
       </c>
       <c r="M159" s="5" t="s">
-        <v>411</v>
+        <v>2502</v>
       </c>
       <c r="N159" s="18"/>
       <c r="O159" s="18"/>
@@ -28357,10 +28402,10 @@
         <v>1889</v>
       </c>
       <c r="J187" s="14" t="s">
-        <v>1102</v>
+        <v>2506</v>
       </c>
       <c r="K187" s="14" t="s">
-        <v>1101</v>
+        <v>2507</v>
       </c>
       <c r="L187" s="14"/>
       <c r="M187" s="14"/>
@@ -35085,16 +35130,16 @@
         <v>1872</v>
       </c>
       <c r="J253" s="14" t="s">
-        <v>1215</v>
+        <v>2503</v>
       </c>
       <c r="K253" s="14" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="L253" s="14" t="s">
-        <v>695</v>
+        <v>2504</v>
       </c>
       <c r="M253" s="14" t="s">
-        <v>696</v>
+        <v>2505</v>
       </c>
       <c r="N253" s="14"/>
       <c r="O253" s="14"/>
@@ -36261,16 +36306,16 @@
         <v>965</v>
       </c>
       <c r="AB264" s="42" t="s">
-        <v>1072</v>
+        <v>2493</v>
       </c>
       <c r="AC264" s="42" t="s">
-        <v>776</v>
+        <v>2489</v>
       </c>
       <c r="AD264" s="42" t="s">
-        <v>769</v>
+        <v>2496</v>
       </c>
       <c r="AE264" s="42" t="s">
-        <v>140</v>
+        <v>2497</v>
       </c>
       <c r="AF264" s="5"/>
       <c r="AG264" s="5"/>

</xml_diff>